<commit_message>
excel dosyasına geliştirmeler yaptım
</commit_message>
<xml_diff>
--- a/temp.xlsx
+++ b/temp.xlsx
@@ -423,6 +423,37 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="15" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="15" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
+    <col width="15" customWidth="1" min="8" max="8"/>
+    <col width="15" customWidth="1" min="9" max="9"/>
+    <col width="15" customWidth="1" min="10" max="10"/>
+    <col width="15" customWidth="1" min="11" max="11"/>
+    <col width="15" customWidth="1" min="12" max="12"/>
+    <col width="15" customWidth="1" min="13" max="13"/>
+    <col width="15" customWidth="1" min="14" max="14"/>
+    <col width="15" customWidth="1" min="15" max="15"/>
+    <col width="15" customWidth="1" min="16" max="16"/>
+    <col width="15" customWidth="1" min="17" max="17"/>
+    <col width="15" customWidth="1" min="18" max="18"/>
+    <col width="15" customWidth="1" min="19" max="19"/>
+    <col width="15" customWidth="1" min="20" max="20"/>
+    <col width="15" customWidth="1" min="21" max="21"/>
+    <col width="15" customWidth="1" min="22" max="22"/>
+    <col width="15" customWidth="1" min="23" max="23"/>
+    <col width="15" customWidth="1" min="24" max="24"/>
+    <col width="15" customWidth="1" min="25" max="25"/>
+    <col width="15" customWidth="1" min="26" max="26"/>
+    <col width="15" customWidth="1" min="27" max="27"/>
+    <col width="15" customWidth="1" min="28" max="28"/>
+    <col width="15" customWidth="1" min="29" max="29"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">

</xml_diff>